<commit_message>
update py scripts after filename func update
</commit_message>
<xml_diff>
--- a/Tutorial/output_mean_median_std.xlsx
+++ b/Tutorial/output_mean_median_std.xlsx
@@ -449,10 +449,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.9819690723183886</v>
+        <v>0.9804946939899589</v>
       </c>
       <c r="C2">
-        <v>0.0203114200037585</v>
+        <v>0.02111941343303251</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -461,16 +461,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>2.65604664760786E-05</v>
+        <v>1.002544042467475E-05</v>
       </c>
       <c r="G2">
-        <v>0.000634746029550483</v>
+        <v>0.0007469541419202988</v>
       </c>
       <c r="H2">
-        <v>0.8418562204076104</v>
+        <v>0.788173738660096</v>
       </c>
       <c r="I2">
-        <v>0.8037827439636921</v>
+        <v>0.6985899269312332</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -478,10 +478,10 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.9823138711697665</v>
+        <v>0.9802013277456616</v>
       </c>
       <c r="C3">
-        <v>0.01984532950318919</v>
+        <v>0.02124921321023904</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -493,13 +493,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.0003915938008713334</v>
+        <v>0.0005123343433966052</v>
       </c>
       <c r="H3">
-        <v>0.7959003413768201</v>
+        <v>0.746236593610306</v>
       </c>
       <c r="I3">
-        <v>0.6334756028871635</v>
+        <v>0.5569000901919152</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -507,10 +507,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.008378299198132795</v>
+        <v>0.00905034109549803</v>
       </c>
       <c r="C4">
-        <v>0.006974947133695278</v>
+        <v>0.007082435258745194</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -519,16 +519,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.0001889755112454919</v>
+        <v>7.495979388161009E-05</v>
       </c>
       <c r="G4">
-        <v>0.000714842558578537</v>
+        <v>0.0007563116016396883</v>
       </c>
       <c r="H4">
-        <v>0.3098726491832139</v>
+        <v>0.2795596909893495</v>
       </c>
       <c r="I4">
-        <v>0.5873727894946082</v>
+        <v>0.493126246596423</v>
       </c>
     </row>
   </sheetData>
@@ -575,10 +575,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.9516248001328913</v>
+        <v>0.9505285992633219</v>
       </c>
       <c r="C2">
-        <v>0.04673231691724285</v>
+        <v>0.0481628733105622</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -590,13 +590,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.002012417701609907</v>
+        <v>0.001991755136295847</v>
       </c>
       <c r="H2">
-        <v>0.9307776610130292</v>
+        <v>0.9935169875817187</v>
       </c>
       <c r="I2">
-        <v>0.9116665095208737</v>
+        <v>1.029937367168262</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -604,10 +604,10 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.9519454925435745</v>
+        <v>0.9510330568296321</v>
       </c>
       <c r="C3">
-        <v>0.04653132816743898</v>
+        <v>0.04840547095840617</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -619,13 +619,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.00207855173494836</v>
+        <v>0.001969193055939746</v>
       </c>
       <c r="H3">
-        <v>0.922559376945658</v>
+        <v>0.9873406510393459</v>
       </c>
       <c r="I3">
-        <v>0.8511174200171766</v>
+        <v>0.9748426250180053</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -633,10 +633,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.01045106470854515</v>
+        <v>0.009685979398901486</v>
       </c>
       <c r="C4">
-        <v>0.004439792999207742</v>
+        <v>0.004094414530504854</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -648,13 +648,13 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.0008426471747546166</v>
+        <v>0.0009343104559375776</v>
       </c>
       <c r="H4">
-        <v>0.213956134652745</v>
+        <v>0.2080728372731967</v>
       </c>
       <c r="I4">
-        <v>0.4255033660054562</v>
+        <v>0.4235300205889955</v>
       </c>
     </row>
   </sheetData>
@@ -701,28 +701,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.9205156343677</v>
+        <v>0.9210671452578729</v>
       </c>
       <c r="C2">
-        <v>0.0749795012310195</v>
+        <v>0.07484834670542642</v>
       </c>
       <c r="D2">
-        <v>0.0008256942967235543</v>
+        <v>0.0006767272104340685</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0003344402414604482</v>
+        <v>0.0005574211738860795</v>
       </c>
       <c r="G2">
-        <v>0.002316621426950536</v>
+        <v>0.002284457111328019</v>
       </c>
       <c r="H2">
-        <v>0.5918057403371705</v>
+        <v>0.5900929104719689</v>
       </c>
       <c r="I2">
-        <v>0.3935809140298243</v>
+        <v>0.4174617901039237</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -730,10 +730,10 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.9204192971028167</v>
+        <v>0.9202187954616341</v>
       </c>
       <c r="C3">
-        <v>0.07496475237022467</v>
+        <v>0.07484162395487856</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -745,13 +745,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.002204465314685201</v>
+        <v>0.002292001681994532</v>
       </c>
       <c r="H3">
-        <v>0.5657865211691311</v>
+        <v>0.5343034131002478</v>
       </c>
       <c r="I3">
-        <v>0.3201354561577427</v>
+        <v>0.2855029087167756</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -759,28 +759,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.006288956432705745</v>
+        <v>0.006749509782455811</v>
       </c>
       <c r="C4">
-        <v>0.003709440147969786</v>
+        <v>0.003487076506787652</v>
       </c>
       <c r="D4">
-        <v>0.001644980601667336</v>
+        <v>0.001264929448071724</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.0008596330024425255</v>
+        <v>0.001400371349777551</v>
       </c>
       <c r="G4">
-        <v>0.001293824333921474</v>
+        <v>0.001160795321446928</v>
       </c>
       <c r="H4">
-        <v>0.2092480035838725</v>
+        <v>0.2644837684096441</v>
       </c>
       <c r="I4">
-        <v>0.275099684901271</v>
+        <v>0.3874999892296863</v>
       </c>
     </row>
   </sheetData>
@@ -827,28 +827,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.8924462060816221</v>
+        <v>0.8909467915408646</v>
       </c>
       <c r="C2">
-        <v>0.09748013233326935</v>
+        <v>0.09826981718768593</v>
       </c>
       <c r="D2">
-        <v>0.0003699498510989908</v>
+        <v>0.000407237501591936</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>7.638670305067734E-05</v>
+        <v>0.0001590283152675463</v>
       </c>
       <c r="G2">
-        <v>0.007040246461558161</v>
+        <v>0.007098195311667276</v>
       </c>
       <c r="H2">
-        <v>0.6187605645799222</v>
+        <v>0.6144091017493711</v>
       </c>
       <c r="I2">
-        <v>0.4102048087354562</v>
+        <v>0.4144231713729987</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -856,10 +856,10 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8924262615771335</v>
+        <v>0.8910814951483663</v>
       </c>
       <c r="C3">
-        <v>0.09705913340775434</v>
+        <v>0.09796615962870754</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -871,13 +871,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.006981799956318089</v>
+        <v>0.007137929119542013</v>
       </c>
       <c r="H3">
-        <v>0.5959750072087142</v>
+        <v>0.588327194415226</v>
       </c>
       <c r="I3">
-        <v>0.3551891857862702</v>
+        <v>0.3461302622541393</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -885,28 +885,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.00539746133836561</v>
+        <v>0.005360470018542446</v>
       </c>
       <c r="C4">
-        <v>0.004365070582276</v>
+        <v>0.004782075550153608</v>
       </c>
       <c r="D4">
-        <v>0.0009959164792198401</v>
+        <v>0.001117154361664795</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.000395430123832958</v>
+        <v>0.0005385346502163977</v>
       </c>
       <c r="G4">
-        <v>0.0006977256701034496</v>
+        <v>0.0006590618484301129</v>
       </c>
       <c r="H4">
-        <v>0.1661816350092133</v>
+        <v>0.1931258736975551</v>
       </c>
       <c r="I4">
-        <v>0.2200422502091548</v>
+        <v>0.2564776693969236</v>
       </c>
     </row>
   </sheetData>
@@ -953,10 +953,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.8782646649734585</v>
+        <v>0.8768849346620484</v>
       </c>
       <c r="C2">
-        <v>0.1237103688886357</v>
+        <v>0.1236260336093482</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -965,16 +965,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>4.991873794869044E-05</v>
+        <v>3.030826661315419E-05</v>
       </c>
       <c r="G2">
-        <v>0.001766815897062621</v>
+        <v>0.001574482790173337</v>
       </c>
       <c r="H2">
-        <v>0.7257194875102805</v>
+        <v>0.6757044307535027</v>
       </c>
       <c r="I2">
-        <v>0.5649945958543107</v>
+        <v>0.4967472555568662</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -982,10 +982,10 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8779486548777997</v>
+        <v>0.8774334371100203</v>
       </c>
       <c r="C3">
-        <v>0.123248391195602</v>
+        <v>0.1239447215296083</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -997,13 +997,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.001819455293819089</v>
+        <v>0.001482346584668842</v>
       </c>
       <c r="H3">
-        <v>0.7149564339565446</v>
+        <v>0.6871177980779859</v>
       </c>
       <c r="I3">
-        <v>0.5111632229509708</v>
+        <v>0.4721684669707958</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1011,10 +1011,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.006510741305286743</v>
+        <v>0.005839523849284185</v>
       </c>
       <c r="C4">
-        <v>0.005315979054753221</v>
+        <v>0.005777157904842808</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1023,16 +1023,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.0003346283355274264</v>
+        <v>0.0002059005774978092</v>
       </c>
       <c r="G4">
-        <v>0.001124456982490767</v>
+        <v>0.0009827128755500966</v>
       </c>
       <c r="H4">
-        <v>0.1967560693097645</v>
+        <v>0.2014362014371931</v>
       </c>
       <c r="I4">
-        <v>0.2984680271054279</v>
+        <v>0.2755773972803012</v>
       </c>
     </row>
   </sheetData>
@@ -1079,28 +1079,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.8065924928867735</v>
+        <v>0.8086143969765271</v>
       </c>
       <c r="C2">
-        <v>0.1603003902375896</v>
+        <v>0.1602747648171917</v>
       </c>
       <c r="D2">
-        <v>0.001144834860444915</v>
+        <v>0.001124212936524953</v>
       </c>
       <c r="E2">
-        <v>0.02864373254751334</v>
+        <v>0.02722234983353262</v>
       </c>
       <c r="F2">
-        <v>0.0002142553084142405</v>
+        <v>0.0003254417992280992</v>
       </c>
       <c r="G2">
-        <v>0.0018685942230329</v>
+        <v>0.001898146728874546</v>
       </c>
       <c r="H2">
-        <v>0.4976614474581713</v>
+        <v>0.5086298223935186</v>
       </c>
       <c r="I2">
-        <v>0.2881511901105325</v>
+        <v>0.3030365732268881</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1108,28 +1108,28 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8068323892322613</v>
+        <v>0.8085324920435435</v>
       </c>
       <c r="C3">
-        <v>0.1599465410845224</v>
+        <v>0.1612849298464366</v>
       </c>
       <c r="D3">
-        <v>0.0003608698637721778</v>
+        <v>0.000395382931832164</v>
       </c>
       <c r="E3">
-        <v>0.02782644428264643</v>
+        <v>0.02757040876659583</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.00185170939704813</v>
+        <v>0.001921677985998357</v>
       </c>
       <c r="H3">
-        <v>0.4743691495387142</v>
+        <v>0.4857835767625893</v>
       </c>
       <c r="I3">
-        <v>0.2251472995892616</v>
+        <v>0.2359877386722556</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1137,28 +1137,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.01256403096464434</v>
+        <v>0.01340511838106049</v>
       </c>
       <c r="C4">
-        <v>0.00570551029716445</v>
+        <v>0.006807665177567592</v>
       </c>
       <c r="D4">
-        <v>0.001455530773753446</v>
+        <v>0.001556251167319811</v>
       </c>
       <c r="E4">
-        <v>0.01296315606759189</v>
+        <v>0.01285893253896804</v>
       </c>
       <c r="F4">
-        <v>0.0009523589537822463</v>
+        <v>0.001184019271675843</v>
       </c>
       <c r="G4">
-        <v>0.0006883675883974569</v>
+        <v>0.0007453497247259198</v>
       </c>
       <c r="H4">
-        <v>0.2022206860912165</v>
+        <v>0.2116130378227949</v>
       </c>
       <c r="I4">
-        <v>0.2193599463322276</v>
+        <v>0.233165306699559</v>
       </c>
     </row>
   </sheetData>
@@ -1205,28 +1205,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.7246172017212558</v>
+        <v>0.7225276718166469</v>
       </c>
       <c r="C2">
-        <v>0.1681825925975229</v>
+        <v>0.1683476697025407</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1038645317225501</v>
+        <v>0.1056918531490265</v>
       </c>
       <c r="F2">
-        <v>8.298959423737342E-05</v>
+        <v>0.0001505186093799428</v>
       </c>
       <c r="G2">
-        <v>0.001395718807421038</v>
+        <v>0.001713610567602463</v>
       </c>
       <c r="H2">
-        <v>0.6006253302743889</v>
+        <v>0.6032203325446551</v>
       </c>
       <c r="I2">
-        <v>0.4018766878516814</v>
+        <v>0.4055468143401456</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1234,28 +1234,28 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.7244806331278918</v>
+        <v>0.7209066823849071</v>
       </c>
       <c r="C3">
-        <v>0.168184116824261</v>
+        <v>0.1679986929826447</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.103544343896274</v>
+        <v>0.1039545710296024</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.001440403346747757</v>
+        <v>0.001790593826712867</v>
       </c>
       <c r="H3">
-        <v>0.5966662387974655</v>
+        <v>0.5774177910919771</v>
       </c>
       <c r="I3">
-        <v>0.3560292076223339</v>
+        <v>0.3334140659682546</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1263,28 +1263,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.014340590026318</v>
+        <v>0.01461677138865287</v>
       </c>
       <c r="C4">
-        <v>0.006140410225281352</v>
+        <v>0.006153242681700203</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.01412871457142256</v>
+        <v>0.01476287531045645</v>
       </c>
       <c r="F4">
-        <v>0.0003254138087629065</v>
+        <v>0.0005586456350725643</v>
       </c>
       <c r="G4">
-        <v>0.0008802098892371085</v>
+        <v>0.0009646668451959455</v>
       </c>
       <c r="H4">
-        <v>0.2038168629448242</v>
+        <v>0.2051657244516217</v>
       </c>
       <c r="I4">
-        <v>0.2596745085424401</v>
+        <v>0.2562449790239522</v>
       </c>
     </row>
   </sheetData>
@@ -1331,28 +1331,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.7077346274716367</v>
+        <v>0.708181185005951</v>
       </c>
       <c r="C2">
-        <v>0.1724737027791001</v>
+        <v>0.1724371912545334</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1103735471902466</v>
+        <v>0.1105563555047107</v>
       </c>
       <c r="F2">
-        <v>0.001410012463597061</v>
+        <v>0.001345672397094279</v>
       </c>
       <c r="G2">
-        <v>0.001137424474911357</v>
+        <v>0.001273726636229345</v>
       </c>
       <c r="H2">
-        <v>0.565889189285373</v>
+        <v>0.5559641398835238</v>
       </c>
       <c r="I2">
-        <v>0.3598760391872515</v>
+        <v>0.351177781255972</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1360,28 +1360,28 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.7078622530653605</v>
+        <v>0.7110669465693369</v>
       </c>
       <c r="C3">
-        <v>0.1723572213170182</v>
+        <v>0.1728993845819258</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.1108271353943358</v>
+        <v>0.1101695916822096</v>
       </c>
       <c r="F3">
-        <v>0.0007686994168280294</v>
+        <v>0.0005424366430353156</v>
       </c>
       <c r="G3">
-        <v>0.00100152752030067</v>
+        <v>0.00108145737859404</v>
       </c>
       <c r="H3">
-        <v>0.5143198412328667</v>
+        <v>0.5432614572229895</v>
       </c>
       <c r="I3">
-        <v>0.2645417079212967</v>
+        <v>0.2951336803803157</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1389,28 +1389,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.01421304953090538</v>
+        <v>0.01360678609333603</v>
       </c>
       <c r="C4">
-        <v>0.005588570773612178</v>
+        <v>0.004975078873867124</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.01446132107085068</v>
+        <v>0.01321033080609342</v>
       </c>
       <c r="F4">
-        <v>0.001592425264205111</v>
+        <v>0.001810870680492265</v>
       </c>
       <c r="G4">
-        <v>0.001001999273376107</v>
+        <v>0.001092250740575729</v>
       </c>
       <c r="H4">
-        <v>0.2001147767556268</v>
+        <v>0.2061715878973304</v>
       </c>
       <c r="I4">
-        <v>0.2429796906649342</v>
+        <v>0.2392256851950242</v>
       </c>
     </row>
   </sheetData>
@@ -1457,28 +1457,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0.6685046874691534</v>
+        <v>0.6673998614153978</v>
       </c>
       <c r="C2">
-        <v>0.1662487656699287</v>
+        <v>0.1658695130496811</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1615763833487698</v>
+        <v>0.1632668539891629</v>
       </c>
       <c r="F2">
-        <v>0.000605543017454374</v>
+        <v>0.0006022375336771106</v>
       </c>
       <c r="G2">
-        <v>0.002030493130115583</v>
+        <v>0.001981173893357759</v>
       </c>
       <c r="H2">
-        <v>0.3670692613471973</v>
+        <v>0.3792595324618012</v>
       </c>
       <c r="I2">
-        <v>0.1551405462109196</v>
+        <v>0.1621825878764195</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1486,28 +1486,28 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.6694716598269435</v>
+        <v>0.6681029752839038</v>
       </c>
       <c r="C3">
-        <v>0.1659142634307919</v>
+        <v>0.1657542500933565</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.1620694393817097</v>
+        <v>0.1622541690094283</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.002119550559192699</v>
+        <v>0.001897682217193756</v>
       </c>
       <c r="H3">
-        <v>0.3462796063447057</v>
+        <v>0.381386846505863</v>
       </c>
       <c r="I3">
-        <v>0.119910172587952</v>
+        <v>0.1454641926694007</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1515,28 +1515,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.01032256077393388</v>
+        <v>0.01217356199633759</v>
       </c>
       <c r="C4">
-        <v>0.005775637522438096</v>
+        <v>0.005193375695966008</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.01104552110563169</v>
+        <v>0.01267891167490279</v>
       </c>
       <c r="F4">
-        <v>0.001111858467022838</v>
+        <v>0.001127419942555604</v>
       </c>
       <c r="G4">
-        <v>0.0004913062624104314</v>
+        <v>0.0005055798376363227</v>
       </c>
       <c r="H4">
-        <v>0.1435505879400071</v>
+        <v>0.1361252947544848</v>
       </c>
       <c r="I4">
-        <v>0.1356946730785947</v>
+        <v>0.1045827009849272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>